<commit_message>
[Commit]       :增加样式 [Modify]       :范伟平 [Code Review]  :范炳林
</commit_message>
<xml_diff>
--- a/简历/简历问题.xlsx
+++ b/简历/简历问题.xlsx
@@ -16,12 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>面试点</t>
   </si>
   <si>
-    <t xml:space="preserve">详细 </t>
+    <t>详细</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>进度</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>难点</t>
   </si>
   <si>
     <t>什么是爬虫，对爬虫的理解</t>
@@ -80,15 +92,31 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -124,13 +152,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -245,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +275,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -278,163 +305,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,154 +577,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1050,107 +1083,119 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="34.125" customWidth="1"/>
     <col min="2" max="2" width="44.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" ht="27" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
+      <c r="A4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Commit]       :增加'' [Modify]       :范伟平 [Code Review]  :范炳林
</commit_message>
<xml_diff>
--- a/简历/简历问题.xlsx
+++ b/简历/简历问题.xlsx
@@ -92,10 +92,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -124,6 +124,37 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,9 +183,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,6 +206,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -170,21 +237,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,59 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -281,6 +281,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -305,19 +329,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,127 +437,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,6 +500,50 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -528,50 +572,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -580,10 +580,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -592,133 +592,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>

</xml_diff>